<commit_message>
Update to 2021_Q1 data
</commit_message>
<xml_diff>
--- a/6) Individual experiments/2020-12-22 - collect data on essential genes/2) Output/Vacuolation_overrepresentation.xlsx
+++ b/6) Individual experiments/2020-12-22 - collect data on essential genes/2) Output/Vacuolation_overrepresentation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\R_root\CRISPR\6) Individual experiments\2020-12-22 - collect data on essential genes\2) Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2418356-5CA1-402C-91EC-ABBA8D1614AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5009A3D-A3A4-4CA7-96FA-6349A7F150C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -801,7 +801,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -841,6 +841,21 @@
     </xf>
     <xf numFmtId="164" fontId="19" fillId="35" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1259,75 +1274,75 @@
       <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5">
-        <v>18171</v>
-      </c>
-      <c r="C2" s="5">
-        <v>2131</v>
-      </c>
-      <c r="D2" s="5">
+      <c r="B2" s="14">
+        <v>18119</v>
+      </c>
+      <c r="C2" s="14">
+        <v>2085</v>
+      </c>
+      <c r="D2" s="14">
         <v>436</v>
       </c>
-      <c r="E2" s="5">
-        <v>15679</v>
-      </c>
-      <c r="F2" s="5">
-        <v>2056</v>
-      </c>
-      <c r="G2" s="5">
+      <c r="E2" s="14">
+        <v>15673</v>
+      </c>
+      <c r="F2" s="14">
+        <v>2010</v>
+      </c>
+      <c r="G2" s="14">
         <v>361</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="15">
         <v>75</v>
       </c>
-      <c r="I2" s="7">
-        <v>1.58428677355962</v>
-      </c>
-      <c r="J2" s="8">
-        <v>1.21334232375152</v>
-      </c>
-      <c r="K2" s="8">
-        <v>2.0461925979440498</v>
-      </c>
-      <c r="L2" s="9">
-        <v>6.5785481343135497E-4</v>
+      <c r="I2" s="16">
+        <v>1.6199226075875801</v>
+      </c>
+      <c r="J2" s="17">
+        <v>1.24048204990668</v>
+      </c>
+      <c r="K2" s="17">
+        <v>2.09234944004079</v>
+      </c>
+      <c r="L2" s="18">
+        <v>3.3745901166429298E-4</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="14">
         <v>16306</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="14">
         <v>1153</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="14">
         <v>396</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="14">
         <v>14798</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="14">
         <v>1112</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="14">
         <v>355</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="15">
         <v>41</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="16">
         <v>1.53686363755309</v>
       </c>
-      <c r="J3" s="8">
+      <c r="J3" s="17">
         <v>1.0778325639889701</v>
       </c>
-      <c r="K3" s="8">
+      <c r="K3" s="17">
         <v>2.1412324181894502</v>
       </c>
-      <c r="L3" s="9">
+      <c r="L3" s="18">
         <v>1.2924831456551499E-2</v>
       </c>
     </row>
@@ -1335,37 +1350,37 @@
       <c r="A4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="14">
         <v>16108</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="14">
         <v>1246</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="14">
         <v>393</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="14">
         <v>14513</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="14">
         <v>1202</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="14">
         <v>349</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="15">
         <v>44</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="16">
         <v>1.5221702021947601</v>
       </c>
-      <c r="J4" s="8">
+      <c r="J4" s="17">
         <v>1.0801770954337899</v>
       </c>
-      <c r="K4" s="8">
+      <c r="K4" s="17">
         <v>2.0999386232897002</v>
       </c>
-      <c r="L4" s="9">
+      <c r="L4" s="18">
         <v>1.26470790086458E-2</v>
       </c>
     </row>
@@ -1373,37 +1388,37 @@
       <c r="A5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="14">
         <v>17688</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="14">
         <v>1625</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="14">
         <v>426</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="14">
         <v>15698</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="14">
         <v>1563</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="14">
         <v>365</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="15">
         <v>62</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="16">
         <v>1.70595203904671</v>
       </c>
-      <c r="J5" s="8">
+      <c r="J5" s="17">
         <v>1.2751494738206799</v>
       </c>
-      <c r="K5" s="8">
+      <c r="K5" s="17">
         <v>2.25063895497181</v>
       </c>
-      <c r="L5" s="9">
+      <c r="L5" s="18">
         <v>3.32824971433592E-4</v>
       </c>
     </row>
@@ -1411,37 +1426,37 @@
       <c r="A6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="14">
         <v>17688</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="14">
         <v>1741</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="14">
         <v>426</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="14">
         <v>15584</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="14">
         <v>1677</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="14">
         <v>363</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="15">
         <v>64</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="16">
         <v>1.63833430747236</v>
       </c>
-      <c r="J6" s="8">
+      <c r="J6" s="17">
         <v>1.2298929771115099</v>
       </c>
-      <c r="K6" s="8">
+      <c r="K6" s="17">
         <v>2.1533555061930598</v>
       </c>
-      <c r="L6" s="9">
+      <c r="L6" s="18">
         <v>6.9397573390724704E-4</v>
       </c>
     </row>
@@ -1449,37 +1464,37 @@
       <c r="A7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="14">
         <v>17470</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="14">
         <v>1839</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="14">
         <v>413</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="14">
         <v>15275</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="14">
         <v>1782</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="14">
         <v>356</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="15">
         <v>57</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="16">
         <v>1.3724234206261601</v>
       </c>
-      <c r="J7" s="8">
+      <c r="J7" s="17">
         <v>1.01443453015301</v>
       </c>
-      <c r="K7" s="8">
+      <c r="K7" s="17">
         <v>1.8280157576270999</v>
       </c>
-      <c r="L7" s="9">
+      <c r="L7" s="18">
         <v>3.4426028288714897E-2</v>
       </c>
     </row>

</xml_diff>